<commit_message>
Consultas hasta la 13, falta 3 y12
</commit_message>
<xml_diff>
--- a/backend/Consulta2.xlsx
+++ b/backend/Consulta2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Espina\Desktop\Compiladores 2\OLC2-Coronavirus-Data-Analysis-With-Machine-Learning\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EB06A6-7844-4D42-BC12-39BF2BEB3EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D63D59-BFB9-49A2-B5CE-F60DE422A778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{509D8F0D-7B5E-44D0-BC14-972074DCFF11}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="198">
   <si>
     <t>Infectados</t>
   </si>
@@ -611,13 +611,28 @@
   </si>
   <si>
     <t>EL RODEO</t>
+  </si>
+  <si>
+    <t>Vacunados</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Hombres</t>
+  </si>
+  <si>
+    <t>Mujer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,12 +651,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFD19A66"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFABB2BF"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -671,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -680,9 +689,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -999,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0982241F-302C-4A7E-BFE3-35BF9F97BC01}">
-  <dimension ref="A1:L181"/>
+  <dimension ref="A1:M190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="M165" sqref="M165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,7 +1019,7 @@
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1032,8 +1038,20 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1052,15 +1070,27 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="2">
@@ -1072,15 +1102,27 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="2">
@@ -1092,15 +1134,27 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2">
@@ -1112,9 +1166,20 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1133,10 +1198,21 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>36</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1155,8 +1231,20 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>40</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1175,8 +1263,20 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>42</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1195,8 +1295,20 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>45</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1215,8 +1327,20 @@
       <c r="F10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>48</v>
+      </c>
+      <c r="H10">
+        <v>62</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1235,8 +1359,20 @@
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>36</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1255,8 +1391,20 @@
       <c r="F12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>52</v>
+      </c>
+      <c r="H12">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1275,8 +1423,20 @@
       <c r="F13">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>54</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1295,8 +1455,20 @@
       <c r="F14">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>56</v>
+      </c>
+      <c r="H14">
+        <v>23</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1315,8 +1487,20 @@
       <c r="F15">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>65</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1335,8 +1519,20 @@
       <c r="F16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>255</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1355,8 +1551,20 @@
       <c r="F17">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>300</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>12</v>
+      </c>
+      <c r="J17">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1375,8 +1583,20 @@
       <c r="F18">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>350</v>
+      </c>
+      <c r="H18" s="1">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1395,8 +1615,20 @@
       <c r="F19">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>400</v>
+      </c>
+      <c r="H19" s="1">
+        <v>9</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1415,8 +1647,20 @@
       <c r="F20">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>450</v>
+      </c>
+      <c r="H20" s="1">
+        <v>9</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1435,8 +1679,20 @@
       <c r="F21">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>500</v>
+      </c>
+      <c r="H21" s="1">
+        <v>13</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1455,8 +1711,20 @@
       <c r="F22">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>395</v>
+      </c>
+      <c r="H22" s="1">
+        <v>22</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1475,8 +1743,20 @@
       <c r="F23">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>419</v>
+      </c>
+      <c r="H23" s="1">
+        <v>23</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1495,8 +1775,20 @@
       <c r="F24">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>443</v>
+      </c>
+      <c r="H24" s="1">
+        <v>26</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1515,8 +1807,20 @@
       <c r="F25">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>468</v>
+      </c>
+      <c r="H25" s="1">
+        <v>27</v>
+      </c>
+      <c r="I25">
+        <v>12</v>
+      </c>
+      <c r="J25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1535,8 +1839,20 @@
       <c r="F26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>492</v>
+      </c>
+      <c r="H26" s="1">
+        <v>35</v>
+      </c>
+      <c r="I26" s="1">
+        <v>41</v>
+      </c>
+      <c r="J26">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1555,8 +1871,20 @@
       <c r="F27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>516</v>
+      </c>
+      <c r="H27" s="1">
+        <v>41</v>
+      </c>
+      <c r="I27" s="1">
+        <v>50</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1575,8 +1903,20 @@
       <c r="F28">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>540</v>
+      </c>
+      <c r="H28" s="1">
+        <v>50</v>
+      </c>
+      <c r="I28" s="1">
+        <v>69</v>
+      </c>
+      <c r="J28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1595,8 +1935,20 @@
       <c r="F29">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>564</v>
+      </c>
+      <c r="H29" s="1">
+        <v>69</v>
+      </c>
+      <c r="I29" s="1">
+        <v>89</v>
+      </c>
+      <c r="J29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1615,8 +1967,20 @@
       <c r="F30">
         <v>41</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>588</v>
+      </c>
+      <c r="H30" s="1">
+        <v>89</v>
+      </c>
+      <c r="I30" s="1">
+        <v>117</v>
+      </c>
+      <c r="J30">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1635,8 +1999,20 @@
       <c r="F31">
         <v>46</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>612</v>
+      </c>
+      <c r="H31" s="1">
+        <v>117</v>
+      </c>
+      <c r="I31" s="1">
+        <v>134</v>
+      </c>
+      <c r="J31">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1655,8 +2031,20 @@
       <c r="F32">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>637</v>
+      </c>
+      <c r="H32" s="1">
+        <v>134</v>
+      </c>
+      <c r="I32" s="1">
+        <v>158</v>
+      </c>
+      <c r="J32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -1675,8 +2063,20 @@
       <c r="F33">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>661</v>
+      </c>
+      <c r="H33" s="1">
+        <v>158</v>
+      </c>
+      <c r="I33" s="1">
+        <v>177</v>
+      </c>
+      <c r="J33">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -1695,8 +2095,20 @@
       <c r="F34">
         <v>46</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>685</v>
+      </c>
+      <c r="H34" s="1">
+        <v>177</v>
+      </c>
+      <c r="I34" s="1">
+        <v>201</v>
+      </c>
+      <c r="J34">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -1715,8 +2127,20 @@
       <c r="F35">
         <v>47</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>709</v>
+      </c>
+      <c r="H35" s="1">
+        <v>201</v>
+      </c>
+      <c r="I35" s="1">
+        <v>231</v>
+      </c>
+      <c r="J35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1735,8 +2159,20 @@
       <c r="F36">
         <v>47</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>733</v>
+      </c>
+      <c r="H36" s="1">
+        <v>231</v>
+      </c>
+      <c r="I36" s="1">
+        <v>263</v>
+      </c>
+      <c r="J36">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -1755,8 +2191,20 @@
       <c r="F37">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>757</v>
+      </c>
+      <c r="H37" s="1">
+        <v>263</v>
+      </c>
+      <c r="I37" s="1">
+        <v>295</v>
+      </c>
+      <c r="J37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -1775,8 +2223,20 @@
       <c r="F38">
         <v>59</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>782</v>
+      </c>
+      <c r="H38" s="1">
+        <v>295</v>
+      </c>
+      <c r="I38" s="1">
+        <v>314</v>
+      </c>
+      <c r="J38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -1795,8 +2255,20 @@
       <c r="F39">
         <v>61</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>806</v>
+      </c>
+      <c r="H39" s="1">
+        <v>314</v>
+      </c>
+      <c r="I39" s="1">
+        <v>330</v>
+      </c>
+      <c r="J39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -1815,8 +2287,20 @@
       <c r="F40">
         <v>64</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>830</v>
+      </c>
+      <c r="H40" s="1">
+        <v>330</v>
+      </c>
+      <c r="I40" s="1">
+        <v>347</v>
+      </c>
+      <c r="J40">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -1835,8 +2319,20 @@
       <c r="F41">
         <v>66</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>854</v>
+      </c>
+      <c r="H41" s="1">
+        <v>347</v>
+      </c>
+      <c r="I41" s="1">
+        <v>375</v>
+      </c>
+      <c r="J41">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -1855,8 +2351,20 @@
       <c r="F42">
         <v>71</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>878</v>
+      </c>
+      <c r="H42" s="1">
+        <v>375</v>
+      </c>
+      <c r="I42" s="1">
+        <v>396</v>
+      </c>
+      <c r="J42">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -1875,8 +2383,20 @@
       <c r="F43">
         <v>75</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>902</v>
+      </c>
+      <c r="H43" s="1">
+        <v>396</v>
+      </c>
+      <c r="I43" s="1">
+        <v>416</v>
+      </c>
+      <c r="J43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -1895,8 +2415,20 @@
       <c r="F44">
         <v>75</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>927</v>
+      </c>
+      <c r="H44" s="1">
+        <v>416</v>
+      </c>
+      <c r="I44" s="1">
+        <v>435</v>
+      </c>
+      <c r="J44">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -1915,8 +2447,20 @@
       <c r="F45">
         <v>76</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>951</v>
+      </c>
+      <c r="H45" s="1">
+        <v>435</v>
+      </c>
+      <c r="I45" s="1">
+        <v>454</v>
+      </c>
+      <c r="J45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1935,9 +2479,20 @@
       <c r="F46">
         <v>82</v>
       </c>
-      <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>975</v>
+      </c>
+      <c r="H46" s="1">
+        <v>454</v>
+      </c>
+      <c r="I46" s="1">
+        <v>467</v>
+      </c>
+      <c r="J46" s="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -1956,8 +2511,20 @@
       <c r="F47">
         <v>83</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>999</v>
+      </c>
+      <c r="H47" s="1">
+        <v>467</v>
+      </c>
+      <c r="I47" s="1">
+        <v>483</v>
+      </c>
+      <c r="J47">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -1976,8 +2543,20 @@
       <c r="F48">
         <v>93</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>1023</v>
+      </c>
+      <c r="H48" s="1">
+        <v>483</v>
+      </c>
+      <c r="I48" s="1">
+        <v>502</v>
+      </c>
+      <c r="J48">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -1996,8 +2575,20 @@
       <c r="F49">
         <v>99</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>1047</v>
+      </c>
+      <c r="H49" s="1">
+        <v>502</v>
+      </c>
+      <c r="I49" s="1">
+        <v>539</v>
+      </c>
+      <c r="J49">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -2016,8 +2607,20 @@
       <c r="F50">
         <v>105</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>1071</v>
+      </c>
+      <c r="H50" s="1">
+        <v>539</v>
+      </c>
+      <c r="I50" s="1">
+        <v>558</v>
+      </c>
+      <c r="J50">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -2036,8 +2639,20 @@
       <c r="F51">
         <v>107</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>1096</v>
+      </c>
+      <c r="H51" s="1">
+        <v>558</v>
+      </c>
+      <c r="I51" s="1">
+        <v>577</v>
+      </c>
+      <c r="J51">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -2056,8 +2671,20 @@
       <c r="F52">
         <v>108</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <v>1120</v>
+      </c>
+      <c r="H52" s="1">
+        <v>577</v>
+      </c>
+      <c r="I52" s="1">
+        <v>595</v>
+      </c>
+      <c r="J52">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -2076,8 +2703,20 @@
       <c r="F53">
         <v>108</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <v>1144</v>
+      </c>
+      <c r="H53" s="1">
+        <v>595</v>
+      </c>
+      <c r="I53" s="1">
+        <v>612</v>
+      </c>
+      <c r="J53">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -2096,8 +2735,20 @@
       <c r="F54">
         <v>116</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>1168</v>
+      </c>
+      <c r="H54" s="1">
+        <v>612</v>
+      </c>
+      <c r="I54" s="1">
+        <v>618</v>
+      </c>
+      <c r="J54">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -2116,8 +2767,20 @@
       <c r="F55">
         <v>121</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <v>1192</v>
+      </c>
+      <c r="H55" s="1">
+        <v>618</v>
+      </c>
+      <c r="I55" s="1">
+        <v>626</v>
+      </c>
+      <c r="J55">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -2136,8 +2799,20 @@
       <c r="F56">
         <v>123</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <v>1216</v>
+      </c>
+      <c r="H56" s="1">
+        <v>626</v>
+      </c>
+      <c r="I56" s="1">
+        <v>642</v>
+      </c>
+      <c r="J56">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -2156,8 +2831,20 @@
       <c r="F57">
         <v>133</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <v>1241</v>
+      </c>
+      <c r="H57" s="1">
+        <v>642</v>
+      </c>
+      <c r="I57" s="1">
+        <v>649</v>
+      </c>
+      <c r="J57">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -2176,8 +2863,20 @@
       <c r="F58">
         <v>134</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <v>1265</v>
+      </c>
+      <c r="H58" s="1">
+        <v>649</v>
+      </c>
+      <c r="I58" s="1">
+        <v>655</v>
+      </c>
+      <c r="J58">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1</v>
       </c>
@@ -2196,8 +2895,20 @@
       <c r="F59">
         <v>138</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <v>1289</v>
+      </c>
+      <c r="H59" s="1">
+        <v>655</v>
+      </c>
+      <c r="I59" s="1">
+        <v>660</v>
+      </c>
+      <c r="J59">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -2216,8 +2927,20 @@
       <c r="F60">
         <v>142</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <v>1313</v>
+      </c>
+      <c r="H60" s="1">
+        <v>660</v>
+      </c>
+      <c r="I60" s="1">
+        <v>662</v>
+      </c>
+      <c r="J60">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -2236,8 +2959,20 @@
       <c r="F61">
         <v>146</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <v>1337</v>
+      </c>
+      <c r="H61" s="1">
+        <v>662</v>
+      </c>
+      <c r="I61" s="1">
+        <v>669</v>
+      </c>
+      <c r="J61">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -2256,8 +2991,20 @@
       <c r="F62">
         <v>147</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <v>1361</v>
+      </c>
+      <c r="H62" s="1">
+        <v>669</v>
+      </c>
+      <c r="I62" s="1">
+        <v>681</v>
+      </c>
+      <c r="J62">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1</v>
       </c>
@@ -2276,8 +3023,20 @@
       <c r="F63">
         <v>151</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <v>1386</v>
+      </c>
+      <c r="H63" s="1">
+        <v>681</v>
+      </c>
+      <c r="I63" s="1">
+        <v>686</v>
+      </c>
+      <c r="J63">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -2296,8 +3055,20 @@
       <c r="F64">
         <v>156</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <v>1410</v>
+      </c>
+      <c r="H64" s="1">
+        <v>686</v>
+      </c>
+      <c r="I64" s="1">
+        <v>687</v>
+      </c>
+      <c r="J64">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -2316,8 +3087,20 @@
       <c r="F65">
         <v>167</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <v>1434</v>
+      </c>
+      <c r="H65" s="1">
+        <v>687</v>
+      </c>
+      <c r="I65" s="1">
+        <v>693</v>
+      </c>
+      <c r="J65">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -2336,8 +3119,20 @@
       <c r="F66">
         <v>174</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <v>1458</v>
+      </c>
+      <c r="H66" s="1">
+        <v>693</v>
+      </c>
+      <c r="I66" s="1">
+        <v>695</v>
+      </c>
+      <c r="J66">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -2356,8 +3151,20 @@
       <c r="F67">
         <v>180</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <v>1482</v>
+      </c>
+      <c r="H67" s="1">
+        <v>695</v>
+      </c>
+      <c r="I67" s="1">
+        <v>697</v>
+      </c>
+      <c r="J67">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1</v>
       </c>
@@ -2376,8 +3183,20 @@
       <c r="F68">
         <v>182</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <v>1506</v>
+      </c>
+      <c r="H68" s="1">
+        <v>697</v>
+      </c>
+      <c r="I68" s="1">
+        <v>705</v>
+      </c>
+      <c r="J68">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1</v>
       </c>
@@ -2396,8 +3215,20 @@
       <c r="F69">
         <v>188</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <v>1530</v>
+      </c>
+      <c r="H69" s="1">
+        <v>705</v>
+      </c>
+      <c r="I69" s="1">
+        <v>713</v>
+      </c>
+      <c r="J69">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -2416,8 +3247,20 @@
       <c r="F70">
         <v>194</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <v>1555</v>
+      </c>
+      <c r="H70" s="1">
+        <v>713</v>
+      </c>
+      <c r="I70" s="1">
+        <v>719</v>
+      </c>
+      <c r="J70">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1</v>
       </c>
@@ -2436,8 +3279,20 @@
       <c r="F71">
         <v>196</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <v>1579</v>
+      </c>
+      <c r="H71" s="1">
+        <v>719</v>
+      </c>
+      <c r="I71" s="1">
+        <v>725</v>
+      </c>
+      <c r="J71">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -2456,8 +3311,20 @@
       <c r="F72">
         <v>199</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <v>1603</v>
+      </c>
+      <c r="H72" s="1">
+        <v>725</v>
+      </c>
+      <c r="I72" s="1">
+        <v>733</v>
+      </c>
+      <c r="J72">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1</v>
       </c>
@@ -2476,8 +3343,20 @@
       <c r="F73">
         <v>201</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73">
+        <v>1627</v>
+      </c>
+      <c r="H73" s="1">
+        <v>733</v>
+      </c>
+      <c r="I73" s="1">
+        <v>739</v>
+      </c>
+      <c r="J73">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1</v>
       </c>
@@ -2496,8 +3375,20 @@
       <c r="F74">
         <v>212</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74">
+        <v>1651</v>
+      </c>
+      <c r="H74" s="1">
+        <v>739</v>
+      </c>
+      <c r="I74" s="1">
+        <v>742</v>
+      </c>
+      <c r="J74">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1</v>
       </c>
@@ -2516,8 +3407,20 @@
       <c r="F75">
         <v>217</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <v>1675</v>
+      </c>
+      <c r="H75" s="1">
+        <v>742</v>
+      </c>
+      <c r="I75" s="1">
+        <v>755</v>
+      </c>
+      <c r="J75">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1</v>
       </c>
@@ -2536,8 +3439,20 @@
       <c r="F76">
         <v>225</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <v>1700</v>
+      </c>
+      <c r="H76" s="1">
+        <v>755</v>
+      </c>
+      <c r="I76" s="1">
+        <v>761</v>
+      </c>
+      <c r="J76">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -2556,8 +3471,20 @@
       <c r="F77">
         <v>234</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <v>1724</v>
+      </c>
+      <c r="H77" s="1">
+        <v>761</v>
+      </c>
+      <c r="I77" s="1">
+        <v>765</v>
+      </c>
+      <c r="J77">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -2576,8 +3503,20 @@
       <c r="F78">
         <v>243</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78">
+        <v>1748</v>
+      </c>
+      <c r="H78" s="1">
+        <v>765</v>
+      </c>
+      <c r="I78" s="1">
+        <v>773</v>
+      </c>
+      <c r="J78">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -2596,8 +3535,20 @@
       <c r="F79">
         <v>248</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79">
+        <v>1772</v>
+      </c>
+      <c r="H79" s="1">
+        <v>773</v>
+      </c>
+      <c r="I79" s="1">
+        <v>780</v>
+      </c>
+      <c r="J79">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1</v>
       </c>
@@ -2616,8 +3567,20 @@
       <c r="F80">
         <v>250</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80">
+        <v>1796</v>
+      </c>
+      <c r="H80" s="1">
+        <v>780</v>
+      </c>
+      <c r="I80" s="1">
+        <v>792</v>
+      </c>
+      <c r="J80">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -2636,8 +3599,20 @@
       <c r="F81">
         <v>258</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81">
+        <v>1820</v>
+      </c>
+      <c r="H81" s="1">
+        <v>792</v>
+      </c>
+      <c r="I81" s="1">
+        <v>801</v>
+      </c>
+      <c r="J81">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1</v>
       </c>
@@ -2656,8 +3631,20 @@
       <c r="F82">
         <v>262</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82">
+        <v>1845</v>
+      </c>
+      <c r="H82" s="1">
+        <v>801</v>
+      </c>
+      <c r="I82" s="1">
+        <v>804</v>
+      </c>
+      <c r="J82">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1</v>
       </c>
@@ -2676,8 +3663,20 @@
       <c r="F83">
         <v>271</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83">
+        <v>1869</v>
+      </c>
+      <c r="H83" s="1">
+        <v>804</v>
+      </c>
+      <c r="I83" s="1">
+        <v>815</v>
+      </c>
+      <c r="J83">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1</v>
       </c>
@@ -2696,8 +3695,20 @@
       <c r="F84">
         <v>290</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84">
+        <v>1893</v>
+      </c>
+      <c r="H84" s="1">
+        <v>815</v>
+      </c>
+      <c r="I84" s="1">
+        <v>830</v>
+      </c>
+      <c r="J84">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -2716,8 +3727,20 @@
       <c r="F85">
         <v>294</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85">
+        <v>1917</v>
+      </c>
+      <c r="H85" s="1">
+        <v>830</v>
+      </c>
+      <c r="I85" s="1">
+        <v>843</v>
+      </c>
+      <c r="J85">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1</v>
       </c>
@@ -2736,8 +3759,20 @@
       <c r="F86">
         <v>306</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86">
+        <v>1941</v>
+      </c>
+      <c r="H86" s="1">
+        <v>843</v>
+      </c>
+      <c r="I86" s="1">
+        <v>853</v>
+      </c>
+      <c r="J86">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1</v>
       </c>
@@ -2756,8 +3791,20 @@
       <c r="F87">
         <v>310</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87">
+        <v>1965</v>
+      </c>
+      <c r="H87" s="1">
+        <v>853</v>
+      </c>
+      <c r="I87" s="1">
+        <v>863</v>
+      </c>
+      <c r="J87">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1</v>
       </c>
@@ -2776,8 +3823,20 @@
       <c r="F88">
         <v>312</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88">
+        <v>1989</v>
+      </c>
+      <c r="H88" s="1">
+        <v>863</v>
+      </c>
+      <c r="I88" s="1">
+        <v>866</v>
+      </c>
+      <c r="J88">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1</v>
       </c>
@@ -2796,8 +3855,20 @@
       <c r="F89">
         <v>322</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89">
+        <v>2014</v>
+      </c>
+      <c r="H89" s="1">
+        <v>866</v>
+      </c>
+      <c r="I89" s="1">
+        <v>882</v>
+      </c>
+      <c r="J89">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1</v>
       </c>
@@ -2816,8 +3887,20 @@
       <c r="F90">
         <v>330</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90">
+        <v>2038</v>
+      </c>
+      <c r="H90" s="1">
+        <v>882</v>
+      </c>
+      <c r="I90" s="1">
+        <v>897</v>
+      </c>
+      <c r="J90">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1</v>
       </c>
@@ -2836,8 +3919,20 @@
       <c r="F91">
         <v>336</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91">
+        <v>2062</v>
+      </c>
+      <c r="H91" s="1">
+        <v>897</v>
+      </c>
+      <c r="I91" s="1">
+        <v>903</v>
+      </c>
+      <c r="J91">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1</v>
       </c>
@@ -2856,8 +3951,20 @@
       <c r="F92">
         <v>343</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92">
+        <v>2086</v>
+      </c>
+      <c r="H92" s="1">
+        <v>903</v>
+      </c>
+      <c r="I92" s="1">
+        <v>911</v>
+      </c>
+      <c r="J92">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>1</v>
       </c>
@@ -2876,8 +3983,20 @@
       <c r="F93">
         <v>349</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93">
+        <v>2110</v>
+      </c>
+      <c r="H93" s="1">
+        <v>911</v>
+      </c>
+      <c r="I93" s="1">
+        <v>918</v>
+      </c>
+      <c r="J93">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1</v>
       </c>
@@ -2896,8 +4015,20 @@
       <c r="F94">
         <v>358</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94">
+        <v>2134</v>
+      </c>
+      <c r="H94" s="1">
+        <v>918</v>
+      </c>
+      <c r="I94" s="1">
+        <v>930</v>
+      </c>
+      <c r="J94">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1</v>
       </c>
@@ -2916,8 +4047,20 @@
       <c r="F95">
         <v>363</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95">
+        <v>2159</v>
+      </c>
+      <c r="H95" s="1">
+        <v>930</v>
+      </c>
+      <c r="I95" s="1">
+        <v>951</v>
+      </c>
+      <c r="J95">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1</v>
       </c>
@@ -2936,8 +4079,20 @@
       <c r="F96">
         <v>395</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96">
+        <v>2183</v>
+      </c>
+      <c r="H96" s="1">
+        <v>951</v>
+      </c>
+      <c r="I96" s="1">
+        <v>956</v>
+      </c>
+      <c r="J96">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>1</v>
       </c>
@@ -2956,8 +4111,20 @@
       <c r="F97">
         <v>405</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97">
+        <v>2207</v>
+      </c>
+      <c r="H97" s="1">
+        <v>956</v>
+      </c>
+      <c r="I97" s="1">
+        <v>984</v>
+      </c>
+      <c r="J97">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1</v>
       </c>
@@ -2976,8 +4143,20 @@
       <c r="F98">
         <v>417</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98">
+        <v>2231</v>
+      </c>
+      <c r="H98" s="1">
+        <v>984</v>
+      </c>
+      <c r="I98" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J98">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>1</v>
       </c>
@@ -2996,8 +4175,20 @@
       <c r="F99">
         <v>426</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99">
+        <v>2255</v>
+      </c>
+      <c r="H99" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I99" s="1">
+        <v>1022</v>
+      </c>
+      <c r="J99">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1</v>
       </c>
@@ -3016,8 +4207,20 @@
       <c r="F100">
         <v>471</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G100">
+        <v>2279</v>
+      </c>
+      <c r="H100" s="1">
+        <v>1022</v>
+      </c>
+      <c r="I100" s="1">
+        <v>1047</v>
+      </c>
+      <c r="J100">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>1</v>
       </c>
@@ -3036,8 +4239,20 @@
       <c r="F101">
         <v>479</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G101">
+        <v>2304</v>
+      </c>
+      <c r="H101" s="1">
+        <v>1047</v>
+      </c>
+      <c r="I101" s="1">
+        <v>1056</v>
+      </c>
+      <c r="J101">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>1</v>
       </c>
@@ -3056,8 +4271,20 @@
       <c r="F102">
         <v>479</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102">
+        <v>2328</v>
+      </c>
+      <c r="H102" s="1">
+        <v>1056</v>
+      </c>
+      <c r="I102" s="1">
+        <v>1084</v>
+      </c>
+      <c r="J102">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>1</v>
       </c>
@@ -3076,8 +4303,20 @@
       <c r="F103">
         <v>485</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G103">
+        <v>2352</v>
+      </c>
+      <c r="H103" s="1">
+        <v>1084</v>
+      </c>
+      <c r="I103" s="1">
+        <v>1105</v>
+      </c>
+      <c r="J103">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1</v>
       </c>
@@ -3096,8 +4335,20 @@
       <c r="F104">
         <v>497</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G104">
+        <v>2376</v>
+      </c>
+      <c r="H104" s="1">
+        <v>1105</v>
+      </c>
+      <c r="I104" s="1">
+        <v>1157</v>
+      </c>
+      <c r="J104">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1</v>
       </c>
@@ -3116,8 +4367,20 @@
       <c r="F105">
         <v>542</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G105">
+        <v>2400</v>
+      </c>
+      <c r="H105" s="1">
+        <v>1157</v>
+      </c>
+      <c r="I105" s="1">
+        <v>1194</v>
+      </c>
+      <c r="J105">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1</v>
       </c>
@@ -3136,8 +4399,20 @@
       <c r="F106">
         <v>591</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G106">
+        <v>2424</v>
+      </c>
+      <c r="H106" s="1">
+        <v>1194</v>
+      </c>
+      <c r="I106" s="1">
+        <v>1228</v>
+      </c>
+      <c r="J106">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1</v>
       </c>
@@ -3156,8 +4431,20 @@
       <c r="F107">
         <v>605</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G107">
+        <v>2448</v>
+      </c>
+      <c r="H107" s="1">
+        <v>1228</v>
+      </c>
+      <c r="I107" s="1">
+        <v>1263</v>
+      </c>
+      <c r="J107">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>1</v>
       </c>
@@ -3176,8 +4463,20 @@
       <c r="F108">
         <v>629</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G108">
+        <v>2473</v>
+      </c>
+      <c r="H108" s="1">
+        <v>1263</v>
+      </c>
+      <c r="I108" s="1">
+        <v>1318</v>
+      </c>
+      <c r="J108">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1</v>
       </c>
@@ -3196,8 +4495,20 @@
       <c r="F109">
         <v>623</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G109">
+        <v>2497</v>
+      </c>
+      <c r="H109" s="1">
+        <v>1318</v>
+      </c>
+      <c r="I109" s="1">
+        <v>1342</v>
+      </c>
+      <c r="J109">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1</v>
       </c>
@@ -3216,8 +4527,20 @@
       <c r="F110">
         <v>656</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G110">
+        <v>2521</v>
+      </c>
+      <c r="H110" s="1">
+        <v>1342</v>
+      </c>
+      <c r="I110" s="1">
+        <v>1375</v>
+      </c>
+      <c r="J110">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1</v>
       </c>
@@ -3236,8 +4559,20 @@
       <c r="F111">
         <v>677</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G111">
+        <v>2545</v>
+      </c>
+      <c r="H111" s="1">
+        <v>1375</v>
+      </c>
+      <c r="I111" s="1">
+        <v>1461</v>
+      </c>
+      <c r="J111">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1</v>
       </c>
@@ -3256,8 +4591,20 @@
       <c r="F112">
         <v>694</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G112">
+        <v>2569</v>
+      </c>
+      <c r="H112" s="1">
+        <v>1461</v>
+      </c>
+      <c r="I112" s="1">
+        <v>1538</v>
+      </c>
+      <c r="J112">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>1</v>
       </c>
@@ -3276,8 +4623,20 @@
       <c r="F113">
         <v>704</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G113">
+        <v>2593</v>
+      </c>
+      <c r="H113" s="1">
+        <v>1538</v>
+      </c>
+      <c r="I113" s="1">
+        <v>1612</v>
+      </c>
+      <c r="J113">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>1</v>
       </c>
@@ -3296,8 +4655,20 @@
       <c r="F114">
         <v>750</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G114">
+        <v>2618</v>
+      </c>
+      <c r="H114" s="1">
+        <v>1612</v>
+      </c>
+      <c r="I114" s="1">
+        <v>1662</v>
+      </c>
+      <c r="J114">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>1</v>
       </c>
@@ -3316,8 +4687,20 @@
       <c r="F115">
         <v>771</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G115">
+        <v>2642</v>
+      </c>
+      <c r="H115" s="1">
+        <v>1662</v>
+      </c>
+      <c r="I115" s="1">
+        <v>1715</v>
+      </c>
+      <c r="J115">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>1</v>
       </c>
@@ -3336,8 +4719,20 @@
       <c r="F116">
         <v>774</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G116">
+        <v>2666</v>
+      </c>
+      <c r="H116" s="1">
+        <v>1715</v>
+      </c>
+      <c r="I116" s="1">
+        <v>1744</v>
+      </c>
+      <c r="J116">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>1</v>
       </c>
@@ -3356,8 +4751,20 @@
       <c r="F117">
         <v>789</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G117">
+        <v>2690</v>
+      </c>
+      <c r="H117" s="1">
+        <v>1744</v>
+      </c>
+      <c r="I117" s="1">
+        <v>1796</v>
+      </c>
+      <c r="J117">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>1</v>
       </c>
@@ -3376,8 +4783,20 @@
       <c r="F118">
         <v>771</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G118">
+        <v>2714</v>
+      </c>
+      <c r="H118" s="1">
+        <v>1796</v>
+      </c>
+      <c r="I118" s="1">
+        <v>1871</v>
+      </c>
+      <c r="J118">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>1</v>
       </c>
@@ -3396,8 +4815,20 @@
       <c r="F119">
         <v>774</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G119">
+        <v>2738</v>
+      </c>
+      <c r="H119" s="1">
+        <v>1871</v>
+      </c>
+      <c r="I119" s="1">
+        <v>1939</v>
+      </c>
+      <c r="J119">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>1</v>
       </c>
@@ -3416,8 +4847,20 @@
       <c r="F120">
         <v>789</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G120">
+        <v>2763</v>
+      </c>
+      <c r="H120" s="1">
+        <v>1939</v>
+      </c>
+      <c r="I120" s="1">
+        <v>2058</v>
+      </c>
+      <c r="J120">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>1</v>
       </c>
@@ -3436,8 +4879,20 @@
       <c r="F121">
         <v>807</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G121">
+        <v>2787</v>
+      </c>
+      <c r="H121" s="1">
+        <v>2058</v>
+      </c>
+      <c r="I121" s="1">
+        <v>2127</v>
+      </c>
+      <c r="J121">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>1</v>
       </c>
@@ -3456,8 +4911,20 @@
       <c r="F122">
         <v>825</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G122">
+        <v>2811</v>
+      </c>
+      <c r="H122" s="1">
+        <v>2127</v>
+      </c>
+      <c r="I122" s="1">
+        <v>2213</v>
+      </c>
+      <c r="J122">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>1</v>
       </c>
@@ -3476,8 +4943,20 @@
       <c r="F123">
         <v>835</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G123">
+        <v>2835</v>
+      </c>
+      <c r="H123" s="1">
+        <v>2213</v>
+      </c>
+      <c r="I123" s="1">
+        <v>2277</v>
+      </c>
+      <c r="J123">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>1</v>
       </c>
@@ -3496,8 +4975,20 @@
       <c r="F124">
         <v>857</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G124">
+        <v>2859</v>
+      </c>
+      <c r="H124" s="1">
+        <v>2277</v>
+      </c>
+      <c r="I124" s="1">
+        <v>2368</v>
+      </c>
+      <c r="J124">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>1</v>
       </c>
@@ -3516,8 +5007,20 @@
       <c r="F125">
         <v>891</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G125">
+        <v>2883</v>
+      </c>
+      <c r="H125" s="1">
+        <v>2368</v>
+      </c>
+      <c r="I125" s="1">
+        <v>2515</v>
+      </c>
+      <c r="J125">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>1</v>
       </c>
@@ -3536,8 +5039,20 @@
       <c r="F126">
         <v>900</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G126">
+        <v>2907</v>
+      </c>
+      <c r="H126" s="1">
+        <v>2515</v>
+      </c>
+      <c r="I126" s="1">
+        <v>2684</v>
+      </c>
+      <c r="J126">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>1</v>
       </c>
@@ -3556,8 +5071,20 @@
       <c r="F127">
         <v>935</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G127">
+        <v>2932</v>
+      </c>
+      <c r="H127" s="1">
+        <v>2684</v>
+      </c>
+      <c r="I127" s="1">
+        <v>2836</v>
+      </c>
+      <c r="J127">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>1</v>
       </c>
@@ -3576,8 +5103,20 @@
       <c r="F128">
         <v>988</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G128">
+        <v>2956</v>
+      </c>
+      <c r="H128" s="1">
+        <v>2836</v>
+      </c>
+      <c r="I128" s="1">
+        <v>2979</v>
+      </c>
+      <c r="J128">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>1</v>
       </c>
@@ -3596,8 +5135,20 @@
       <c r="F129">
         <v>1006</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G129">
+        <v>2980</v>
+      </c>
+      <c r="H129" s="1">
+        <v>2979</v>
+      </c>
+      <c r="I129" s="1">
+        <v>3130</v>
+      </c>
+      <c r="J129">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>1</v>
       </c>
@@ -3616,8 +5167,20 @@
       <c r="F130">
         <v>1011</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G130">
+        <v>3004</v>
+      </c>
+      <c r="H130" s="1">
+        <v>3130</v>
+      </c>
+      <c r="I130" s="1">
+        <v>3269</v>
+      </c>
+      <c r="J130">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>1</v>
       </c>
@@ -3636,8 +5199,20 @@
       <c r="F131">
         <v>1061</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G131">
+        <v>3028</v>
+      </c>
+      <c r="H131" s="1">
+        <v>3269</v>
+      </c>
+      <c r="I131" s="1">
+        <v>3459</v>
+      </c>
+      <c r="J131">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>1</v>
       </c>
@@ -3656,8 +5231,20 @@
       <c r="F132">
         <v>1098</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G132">
+        <v>3052</v>
+      </c>
+      <c r="H132" s="1">
+        <v>3459</v>
+      </c>
+      <c r="I132" s="1">
+        <v>3753</v>
+      </c>
+      <c r="J132">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>1</v>
       </c>
@@ -3676,8 +5263,20 @@
       <c r="F133">
         <v>1116</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G133">
+        <v>3077</v>
+      </c>
+      <c r="H133" s="1">
+        <v>3753</v>
+      </c>
+      <c r="I133" s="1">
+        <v>4023</v>
+      </c>
+      <c r="J133">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>1</v>
       </c>
@@ -3696,8 +5295,20 @@
       <c r="F134">
         <v>1166</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G134">
+        <v>3101</v>
+      </c>
+      <c r="H134" s="1">
+        <v>4023</v>
+      </c>
+      <c r="I134" s="1">
+        <v>4311</v>
+      </c>
+      <c r="J134">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>1</v>
       </c>
@@ -3716,8 +5327,20 @@
       <c r="F135">
         <v>1214</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G135">
+        <v>3125</v>
+      </c>
+      <c r="H135" s="1">
+        <v>4311</v>
+      </c>
+      <c r="I135" s="1">
+        <v>4621</v>
+      </c>
+      <c r="J135">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>1</v>
       </c>
@@ -3736,8 +5359,20 @@
       <c r="F136">
         <v>1259</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G136">
+        <v>3149</v>
+      </c>
+      <c r="H136" s="1">
+        <v>4621</v>
+      </c>
+      <c r="I136" s="1">
+        <v>4996</v>
+      </c>
+      <c r="J136">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>1</v>
       </c>
@@ -3756,8 +5391,20 @@
       <c r="F137">
         <v>1312</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G137">
+        <v>3173</v>
+      </c>
+      <c r="H137" s="1">
+        <v>4996</v>
+      </c>
+      <c r="I137" s="1">
+        <v>5241</v>
+      </c>
+      <c r="J137">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>1</v>
       </c>
@@ -3776,8 +5423,20 @@
       <c r="F138">
         <v>1337</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G138">
+        <v>3197</v>
+      </c>
+      <c r="H138" s="1">
+        <v>5241</v>
+      </c>
+      <c r="I138" s="1">
+        <v>5486</v>
+      </c>
+      <c r="J138">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>1</v>
       </c>
@@ -3796,8 +5455,20 @@
       <c r="F139">
         <v>1368</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G139">
+        <v>3222</v>
+      </c>
+      <c r="H139" s="1">
+        <v>5486</v>
+      </c>
+      <c r="I139" s="1">
+        <v>5836</v>
+      </c>
+      <c r="J139">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>1</v>
       </c>
@@ -3816,8 +5487,20 @@
       <c r="F140">
         <v>1377</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G140">
+        <v>3246</v>
+      </c>
+      <c r="H140" s="1">
+        <v>5836</v>
+      </c>
+      <c r="I140" s="1">
+        <v>6485</v>
+      </c>
+      <c r="J140">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>1</v>
       </c>
@@ -3836,8 +5519,20 @@
       <c r="F141">
         <v>1384</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G141">
+        <v>3270</v>
+      </c>
+      <c r="H141" s="1">
+        <v>6485</v>
+      </c>
+      <c r="I141" s="1">
+        <v>6845</v>
+      </c>
+      <c r="J141">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>1</v>
       </c>
@@ -3856,9 +5551,21 @@
       <c r="F142">
         <v>1400</v>
       </c>
-      <c r="J142" s="4"/>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G142">
+        <v>3294</v>
+      </c>
+      <c r="H142" s="1">
+        <v>6845</v>
+      </c>
+      <c r="I142" s="1">
+        <v>7231</v>
+      </c>
+      <c r="J142">
+        <v>25</v>
+      </c>
+      <c r="K142" s="4"/>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>1</v>
       </c>
@@ -3877,8 +5584,20 @@
       <c r="F143">
         <v>1423</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G143">
+        <v>3318</v>
+      </c>
+      <c r="H143" s="1">
+        <v>7231</v>
+      </c>
+      <c r="I143" s="1">
+        <v>7596</v>
+      </c>
+      <c r="J143">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>1</v>
       </c>
@@ -3897,8 +5616,20 @@
       <c r="F144">
         <v>1446</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G144">
+        <v>3342</v>
+      </c>
+      <c r="H144" s="1">
+        <v>7596</v>
+      </c>
+      <c r="I144" s="1">
+        <v>8036</v>
+      </c>
+      <c r="J144">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>1</v>
       </c>
@@ -3917,8 +5648,20 @@
       <c r="F145">
         <v>1465</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G145">
+        <v>3366</v>
+      </c>
+      <c r="H145" s="1">
+        <v>8036</v>
+      </c>
+      <c r="I145" s="1">
+        <v>8482</v>
+      </c>
+      <c r="J145">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>1</v>
       </c>
@@ -3937,8 +5680,20 @@
       <c r="F146">
         <v>1476</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G146">
+        <v>3391</v>
+      </c>
+      <c r="H146" s="1">
+        <v>8482</v>
+      </c>
+      <c r="I146" s="1">
+        <v>8986</v>
+      </c>
+      <c r="J146">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>1</v>
       </c>
@@ -3957,8 +5712,20 @@
       <c r="F147">
         <v>1495</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G147">
+        <v>3415</v>
+      </c>
+      <c r="H147" s="1">
+        <v>8986</v>
+      </c>
+      <c r="I147" s="1">
+        <v>9546</v>
+      </c>
+      <c r="J147">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>1</v>
       </c>
@@ -3977,8 +5744,20 @@
       <c r="F148">
         <v>1506</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G148">
+        <v>3439</v>
+      </c>
+      <c r="H148" s="1">
+        <v>9546</v>
+      </c>
+      <c r="I148" s="1">
+        <v>9969</v>
+      </c>
+      <c r="J148">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>1</v>
       </c>
@@ -3997,8 +5776,20 @@
       <c r="F149">
         <v>1515</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G149">
+        <v>3463</v>
+      </c>
+      <c r="H149" s="1">
+        <v>9969</v>
+      </c>
+      <c r="I149" s="1">
+        <v>10551</v>
+      </c>
+      <c r="J149">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>1</v>
       </c>
@@ -4017,8 +5808,20 @@
       <c r="F150">
         <v>1533</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G150">
+        <v>3487</v>
+      </c>
+      <c r="H150" s="1">
+        <v>10551</v>
+      </c>
+      <c r="I150" s="1">
+        <v>11114</v>
+      </c>
+      <c r="J150">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>1</v>
       </c>
@@ -4037,8 +5840,20 @@
       <c r="F151">
         <v>1542</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G151">
+        <v>3511</v>
+      </c>
+      <c r="H151" s="1">
+        <v>11114</v>
+      </c>
+      <c r="I151" s="1">
+        <v>11534</v>
+      </c>
+      <c r="J151">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>1</v>
       </c>
@@ -4057,8 +5872,20 @@
       <c r="F152">
         <v>1548</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G152">
+        <v>3536</v>
+      </c>
+      <c r="H152" s="1">
+        <v>11534</v>
+      </c>
+      <c r="I152" s="1">
+        <v>11811</v>
+      </c>
+      <c r="J152">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>1</v>
       </c>
@@ -4077,8 +5904,20 @@
       <c r="F153">
         <v>1567</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G153">
+        <v>3560</v>
+      </c>
+      <c r="H153" s="1">
+        <v>11811</v>
+      </c>
+      <c r="I153" s="1">
+        <v>12361</v>
+      </c>
+      <c r="J153">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>4</v>
       </c>
@@ -4097,8 +5936,20 @@
       <c r="F154">
         <v>1575</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G154">
+        <v>3584</v>
+      </c>
+      <c r="H154" s="1">
+        <v>12361</v>
+      </c>
+      <c r="I154" s="1">
+        <v>13129</v>
+      </c>
+      <c r="J154">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>4</v>
       </c>
@@ -4117,8 +5968,20 @@
       <c r="F155">
         <v>1583</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G155">
+        <v>3608</v>
+      </c>
+      <c r="H155" s="1">
+        <v>13129</v>
+      </c>
+      <c r="I155" s="1">
+        <v>13669</v>
+      </c>
+      <c r="J155">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>4</v>
       </c>
@@ -4137,8 +6000,20 @@
       <c r="F156">
         <v>1593</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G156">
+        <v>3632</v>
+      </c>
+      <c r="H156" s="1">
+        <v>13669</v>
+      </c>
+      <c r="I156" s="1">
+        <v>14600</v>
+      </c>
+      <c r="J156">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>4</v>
       </c>
@@ -4157,9 +6032,20 @@
       <c r="F157">
         <v>1608</v>
       </c>
-      <c r="H157" s="5"/>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G157">
+        <v>3656</v>
+      </c>
+      <c r="H157" s="1">
+        <v>14600</v>
+      </c>
+      <c r="I157" s="1">
+        <v>15229</v>
+      </c>
+      <c r="J157">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>4</v>
       </c>
@@ -4178,8 +6064,20 @@
       <c r="F158">
         <v>1619</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G158">
+        <v>3681</v>
+      </c>
+      <c r="H158" s="1">
+        <v>15229</v>
+      </c>
+      <c r="I158" s="1">
+        <v>15841</v>
+      </c>
+      <c r="J158">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>4</v>
       </c>
@@ -4198,8 +6096,20 @@
       <c r="F159">
         <v>1632</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G159">
+        <v>3705</v>
+      </c>
+      <c r="H159" s="1">
+        <v>15841</v>
+      </c>
+      <c r="I159" s="1">
+        <v>16344</v>
+      </c>
+      <c r="J159">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>4</v>
       </c>
@@ -4218,8 +6128,20 @@
       <c r="F160">
         <v>1643</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G160">
+        <v>3729</v>
+      </c>
+      <c r="H160" s="1">
+        <v>16344</v>
+      </c>
+      <c r="I160" s="1">
+        <v>16800</v>
+      </c>
+      <c r="J160">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>4</v>
       </c>
@@ -4238,8 +6160,20 @@
       <c r="F161">
         <v>1654</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G161">
+        <v>3753</v>
+      </c>
+      <c r="H161" s="1">
+        <v>16800</v>
+      </c>
+      <c r="I161" s="1">
+        <v>17290</v>
+      </c>
+      <c r="J161">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>4</v>
       </c>
@@ -4258,8 +6192,20 @@
       <c r="F162">
         <v>1683</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G162">
+        <v>3777</v>
+      </c>
+      <c r="H162" s="1">
+        <v>17290</v>
+      </c>
+      <c r="I162" s="1">
+        <v>17820</v>
+      </c>
+      <c r="J162">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>4</v>
       </c>
@@ -4278,8 +6224,20 @@
       <c r="F163">
         <v>1703</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G163">
+        <v>3801</v>
+      </c>
+      <c r="H163" s="1">
+        <v>17820</v>
+      </c>
+      <c r="I163" s="1">
+        <v>18187</v>
+      </c>
+      <c r="J163">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>4</v>
       </c>
@@ -4298,8 +6256,20 @@
       <c r="F164">
         <v>1747</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G164">
+        <v>3825</v>
+      </c>
+      <c r="H164" s="1">
+        <v>18187</v>
+      </c>
+      <c r="I164" s="1">
+        <v>18975</v>
+      </c>
+      <c r="J164">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>4</v>
       </c>
@@ -4318,8 +6288,20 @@
       <c r="F165">
         <v>1803</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G165">
+        <v>3850</v>
+      </c>
+      <c r="H165" s="1">
+        <v>18975</v>
+      </c>
+      <c r="I165" s="1">
+        <v>19402</v>
+      </c>
+      <c r="J165">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>4</v>
       </c>
@@ -4338,8 +6320,20 @@
       <c r="F166">
         <v>1827</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G166">
+        <v>3874</v>
+      </c>
+      <c r="H166" s="1">
+        <v>19402</v>
+      </c>
+      <c r="I166">
+        <v>1842</v>
+      </c>
+      <c r="J166">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>4</v>
       </c>
@@ -4358,8 +6352,20 @@
       <c r="F167">
         <v>1842</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G167">
+        <v>3898</v>
+      </c>
+      <c r="H167">
+        <v>3898</v>
+      </c>
+      <c r="I167">
+        <v>1858</v>
+      </c>
+      <c r="J167">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>4</v>
       </c>
@@ -4378,8 +6384,20 @@
       <c r="F168">
         <v>1858</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G168">
+        <v>3922</v>
+      </c>
+      <c r="H168">
+        <v>3922</v>
+      </c>
+      <c r="I168">
+        <v>1873</v>
+      </c>
+      <c r="J168">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>4</v>
       </c>
@@ -4398,8 +6416,20 @@
       <c r="F169">
         <v>1873</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G169">
+        <v>3946</v>
+      </c>
+      <c r="H169">
+        <v>3946</v>
+      </c>
+      <c r="I169">
+        <v>1888</v>
+      </c>
+      <c r="J169">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>4</v>
       </c>
@@ -4418,8 +6448,20 @@
       <c r="F170">
         <v>1888</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G170">
+        <v>3970</v>
+      </c>
+      <c r="H170">
+        <v>3970</v>
+      </c>
+      <c r="I170">
+        <v>1924</v>
+      </c>
+      <c r="J170">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>4</v>
       </c>
@@ -4438,8 +6480,20 @@
       <c r="F171">
         <v>1924</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G171">
+        <v>3995</v>
+      </c>
+      <c r="H171">
+        <v>3995</v>
+      </c>
+      <c r="I171">
+        <v>363</v>
+      </c>
+      <c r="J171">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>4</v>
       </c>
@@ -4458,8 +6512,20 @@
       <c r="F172">
         <v>363</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G172">
+        <v>4019</v>
+      </c>
+      <c r="H172">
+        <v>4019</v>
+      </c>
+      <c r="I172">
+        <v>395</v>
+      </c>
+      <c r="J172">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>4</v>
       </c>
@@ -4478,8 +6544,20 @@
       <c r="F173">
         <v>395</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G173">
+        <v>4043</v>
+      </c>
+      <c r="H173">
+        <v>4043</v>
+      </c>
+      <c r="I173">
+        <v>405</v>
+      </c>
+      <c r="J173">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>4</v>
       </c>
@@ -4498,8 +6576,20 @@
       <c r="F174">
         <v>405</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G174">
+        <v>4067</v>
+      </c>
+      <c r="H174">
+        <v>4067</v>
+      </c>
+      <c r="I174">
+        <v>417</v>
+      </c>
+      <c r="J174">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>4</v>
       </c>
@@ -4518,8 +6608,20 @@
       <c r="F175">
         <v>417</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G175">
+        <v>4091</v>
+      </c>
+      <c r="H175">
+        <v>4091</v>
+      </c>
+      <c r="I175">
+        <v>426</v>
+      </c>
+      <c r="J175">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>4</v>
       </c>
@@ -4538,8 +6640,20 @@
       <c r="F176">
         <v>426</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G176">
+        <v>4115</v>
+      </c>
+      <c r="H176">
+        <v>4115</v>
+      </c>
+      <c r="I176">
+        <v>471</v>
+      </c>
+      <c r="J176">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>4</v>
       </c>
@@ -4558,8 +6672,20 @@
       <c r="F177">
         <v>471</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G177">
+        <v>4140</v>
+      </c>
+      <c r="H177">
+        <v>4140</v>
+      </c>
+      <c r="I177">
+        <v>479</v>
+      </c>
+      <c r="J177">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>4</v>
       </c>
@@ -4578,8 +6704,20 @@
       <c r="F178">
         <v>479</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G178">
+        <v>4164</v>
+      </c>
+      <c r="H178">
+        <v>4164</v>
+      </c>
+      <c r="I178">
+        <v>479</v>
+      </c>
+      <c r="J178">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>4</v>
       </c>
@@ -4598,8 +6736,20 @@
       <c r="F179">
         <v>479</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G179">
+        <v>4188</v>
+      </c>
+      <c r="H179">
+        <v>4188</v>
+      </c>
+      <c r="I179">
+        <v>485</v>
+      </c>
+      <c r="J179">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>4</v>
       </c>
@@ -4618,8 +6768,20 @@
       <c r="F180">
         <v>485</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G180">
+        <v>4212</v>
+      </c>
+      <c r="H180">
+        <v>4212</v>
+      </c>
+      <c r="I180">
+        <v>497</v>
+      </c>
+      <c r="J180">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>4</v>
       </c>
@@ -4638,6 +6800,45 @@
       <c r="F181">
         <v>497</v>
       </c>
+      <c r="G181">
+        <v>4236</v>
+      </c>
+      <c r="H181">
+        <v>4236</v>
+      </c>
+      <c r="I181" t="s">
+        <v>194</v>
+      </c>
+      <c r="J181">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J182" s="3"/>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J183" s="3"/>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J184" s="3"/>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J185" s="3"/>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J186" s="3"/>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J187" s="3"/>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J188" s="3"/>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J189" s="3"/>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J190" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>